<commit_message>
update with descriptions, improved toggle function
</commit_message>
<xml_diff>
--- a/images/fulls/PhotoIndex.xlsx
+++ b/images/fulls/PhotoIndex.xlsx
@@ -8,33 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltsai\Documents\Personal\Github\VirginiaWebsite\VirginiaWebsite\images\fulls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE471507-D52D-4B05-8273-66A372F2AAC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030527BE-0F34-4F89-BF6C-31932F8B7D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="4035" windowWidth="17280" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj8o5TPxwe9D/z+GZ5yFej/gzPLlQ=="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+  <si>
+    <t>Image Name</t>
+  </si>
+  <si>
+    <t>Subtitle</t>
+  </si>
   <si>
     <t>Tag 1</t>
   </si>
@@ -60,30 +52,24 @@
     <t>D</t>
   </si>
   <si>
+    <t>img (1).jpg</t>
+  </si>
+  <si>
+    <t>Portrait</t>
+  </si>
+  <si>
+    <t>img (2).jpg</t>
+  </si>
+  <si>
+    <t>Landscape</t>
+  </si>
+  <si>
+    <t>img (3).jpg</t>
+  </si>
+  <si>
     <t>Still</t>
   </si>
   <si>
-    <t>Landscape</t>
-  </si>
-  <si>
-    <t>Portrait</t>
-  </si>
-  <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
-    <t>Image Name</t>
-  </si>
-  <si>
-    <t>img (1).jpg</t>
-  </si>
-  <si>
-    <t>img (2).jpg</t>
-  </si>
-  <si>
-    <t>img (3).jpg</t>
-  </si>
-  <si>
     <t>img (4).jpg</t>
   </si>
   <si>
@@ -96,15 +82,15 @@
     <t>img (7).jpg</t>
   </si>
   <si>
-    <t>img (8).jpg</t>
-  </si>
-  <si>
     <t>img (9).jpg</t>
   </si>
   <si>
     <t>img (10).jpg</t>
   </si>
   <si>
+    <t>Street</t>
+  </si>
+  <si>
     <t>img (11).jpg</t>
   </si>
   <si>
@@ -162,6 +148,9 @@
     <t>img (29).jpg</t>
   </si>
   <si>
+    <t>img (30).jpg</t>
+  </si>
+  <si>
     <t>img (31).jpg</t>
   </si>
   <si>
@@ -189,131 +178,104 @@
     <t>img (39).jpg</t>
   </si>
   <si>
-    <t>img (30).jpg</t>
-  </si>
-  <si>
-    <t>Image 1</t>
-  </si>
-  <si>
-    <t>Image 2</t>
-  </si>
-  <si>
-    <t>Image 3</t>
-  </si>
-  <si>
-    <t>Image 4</t>
-  </si>
-  <si>
-    <t>Image 5</t>
-  </si>
-  <si>
-    <t>Image 6</t>
-  </si>
-  <si>
-    <t>Image 7</t>
-  </si>
-  <si>
-    <t>Image 8</t>
-  </si>
-  <si>
-    <t>Image 9</t>
-  </si>
-  <si>
-    <t>Image 10</t>
-  </si>
-  <si>
-    <t>Image 11</t>
-  </si>
-  <si>
-    <t>Image 12</t>
-  </si>
-  <si>
-    <t>Image 13</t>
-  </si>
-  <si>
-    <t>Image 14</t>
-  </si>
-  <si>
-    <t>Image 15</t>
-  </si>
-  <si>
-    <t>Image 16</t>
-  </si>
-  <si>
-    <t>Image 17</t>
-  </si>
-  <si>
-    <t>Image 18</t>
-  </si>
-  <si>
-    <t>Image 19</t>
-  </si>
-  <si>
-    <t>Image 20</t>
-  </si>
-  <si>
-    <t>Image 21</t>
-  </si>
-  <si>
-    <t>Image 22</t>
-  </si>
-  <si>
-    <t>Image 23</t>
-  </si>
-  <si>
-    <t>Image 24</t>
-  </si>
-  <si>
-    <t>Image 25</t>
-  </si>
-  <si>
-    <t>Image 26</t>
-  </si>
-  <si>
-    <t>Image 27</t>
-  </si>
-  <si>
-    <t>Image 28</t>
-  </si>
-  <si>
-    <t>Image 29</t>
-  </si>
-  <si>
-    <t>Image 30</t>
-  </si>
-  <si>
-    <t>Image 31</t>
-  </si>
-  <si>
-    <t>Image 32</t>
-  </si>
-  <si>
-    <t>Image 33</t>
-  </si>
-  <si>
-    <t>Image 34</t>
-  </si>
-  <si>
-    <t>Image 35</t>
-  </si>
-  <si>
-    <t>Image 36</t>
-  </si>
-  <si>
-    <t>Image 37</t>
-  </si>
-  <si>
-    <t>Image 38</t>
-  </si>
-  <si>
-    <t>Image 39</t>
+    <t>Family Portraits</t>
+  </si>
+  <si>
+    <t>beauty in grocery store flowers</t>
+  </si>
+  <si>
+    <t>Patriotism in the North End</t>
+  </si>
+  <si>
+    <t>North Carolina Mountains</t>
+  </si>
+  <si>
+    <t>Boston's North Star</t>
+  </si>
+  <si>
+    <t>Boston Spring Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring: the perfect time for portraits! </t>
+  </si>
+  <si>
+    <t>Quinsigamond - Worcester, MA</t>
+  </si>
+  <si>
+    <t>Fenway Area Photography</t>
+  </si>
+  <si>
+    <t>Movements with slow shutter speeds</t>
+  </si>
+  <si>
+    <t>Dusk Light - The perfect opportunity!</t>
+  </si>
+  <si>
+    <t>Street Photography at Dusk</t>
+  </si>
+  <si>
+    <t>Regatta Photography</t>
+  </si>
+  <si>
+    <t>Beantown</t>
+  </si>
+  <si>
+    <t>Boston Lights</t>
+  </si>
+  <si>
+    <t>Two Paths</t>
+  </si>
+  <si>
+    <t>Sunsets</t>
+  </si>
+  <si>
+    <t>Fresh Snowfall - Brookline, MA</t>
+  </si>
+  <si>
+    <t>Kenmore Lights</t>
+  </si>
+  <si>
+    <t>Butterfly Exhibit - Over the Charles</t>
+  </si>
+  <si>
+    <t>The Lights</t>
+  </si>
+  <si>
+    <t>Life in Boston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Photography  </t>
+  </si>
+  <si>
+    <t>Boston's Hidden Gardens</t>
+  </si>
+  <si>
+    <t>Never too Bald for Bubbles</t>
+  </si>
+  <si>
+    <t>Simple Happiness</t>
+  </si>
+  <si>
+    <t>Relaxed in Miami</t>
+  </si>
+  <si>
+    <t>Destin, FL</t>
+  </si>
+  <si>
+    <t>Off the Coast of Pensacola, FL</t>
+  </si>
+  <si>
+    <t>Georgia Gardening</t>
+  </si>
+  <si>
+    <t>The Only Time of Year a Hat Full of Water is Acceptable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,24 +291,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -370,16 +314,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,16 +538,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1000"/>
+  <dimension ref="A1:T999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="7.125" customWidth="1"/>
     <col min="4" max="4" width="8.875" customWidth="1"/>
     <col min="5" max="6" width="4.875" customWidth="1"/>
@@ -616,658 +560,678 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="K48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="K58" s="1"/>
     </row>
     <row r="59" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
     </row>
     <row r="67" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
     </row>
     <row r="69" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
     </row>
     <row r="70" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="3"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
-    </row>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2195,9 +2159,7 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>